<commit_message>
[chage logic]: 지정 단어군 변동
</commit_message>
<xml_diff>
--- a/HPU_dict.xlsx
+++ b/HPU_dict.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\users\Desktop\Junhwi\국토연구원\HPU_Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\wnsgnl\Desktop\paper_master2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D4FB67-4788-4191-98A6-6488B307D253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37D2DF2-40C7-414E-B70D-DB451C8186B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{17033906-44DF-451E-ABB7-AE170C71C853}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{17033906-44DF-451E-ABB7-AE170C71C853}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="124">
   <si>
     <t>tag</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -69,6 +69,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>부동산시장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부동산 시장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부동산가격</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부동산 가격</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아파트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>U-A</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -149,6 +169,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t xml:space="preserve">세금 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>취득세</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -169,11 +193,343 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>제정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">법안 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>법률</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한은</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">금융위원회 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금융 위원회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">금융위 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금융통화위원회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금융 통화 위원회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">금융통화 위원회 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금통위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기획재정부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기획 재정부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기재부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재정경제부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재정 경제부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재경부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>청와대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당국</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중앙은행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중앙 은행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">국무회의 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국무 회의</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통화정책</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>통화 정책</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대책</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주택정책</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주택 정책</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부동산 대책</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부동산대책</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주택법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모기지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모기지론</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LTV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ltv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DTI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dti</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DSR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dsr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이자율</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대출금리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대출 금리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대출 이자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대출이자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부동산세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>거래세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양도소득세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양도 소득세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>보유세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재산세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종합부동산세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종부세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>종합 부동산세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국토교통부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국토 교통부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국토부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국세청</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>건설교통부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>건설 교통부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>건교부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상속</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>증여</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다주택자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>투기지역</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>투기과열지구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>투기 과열지구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>투기과열 지구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>투기 과열 지구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미분양</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분양</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>청약</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재건축</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>재개발</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공급</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조정대상지역</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조정 대상지역</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조정 대상 지역</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>word</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>세금</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -556,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5237A7CA-675B-4995-AE5A-4D0BBE0D4412}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -572,7 +928,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -625,47 +981,47 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -673,103 +1029,103 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>27</v>
@@ -777,7 +1133,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
         <v>28</v>
@@ -785,42 +1141,754 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>24</v>
+      </c>
+      <c r="B54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>24</v>
+      </c>
+      <c r="B58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>24</v>
+      </c>
+      <c r="B59" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>24</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>24</v>
+      </c>
+      <c r="B61" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>24</v>
+      </c>
+      <c r="B65" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>24</v>
+      </c>
+      <c r="B68" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>24</v>
+      </c>
+      <c r="B69" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>24</v>
+      </c>
+      <c r="B70" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>24</v>
+      </c>
+      <c r="B71" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>24</v>
+      </c>
+      <c r="B72" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>24</v>
+      </c>
+      <c r="B73" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>24</v>
+      </c>
+      <c r="B74" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>24</v>
+      </c>
+      <c r="B75" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>24</v>
+      </c>
+      <c r="B76" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>24</v>
+      </c>
+      <c r="B77" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>24</v>
+      </c>
+      <c r="B78" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>24</v>
+      </c>
+      <c r="B79" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>24</v>
+      </c>
+      <c r="B81" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>24</v>
+      </c>
+      <c r="B82" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>24</v>
+      </c>
+      <c r="B83" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>24</v>
+      </c>
+      <c r="B84" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>24</v>
+      </c>
+      <c r="B85" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>24</v>
+      </c>
+      <c r="B86" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>24</v>
+      </c>
+      <c r="B87" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>24</v>
+      </c>
+      <c r="B88" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>24</v>
+      </c>
+      <c r="B89" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>24</v>
+      </c>
+      <c r="B90" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>24</v>
+      </c>
+      <c r="B91" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>24</v>
+      </c>
+      <c r="B92" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>24</v>
+      </c>
+      <c r="B93" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>24</v>
+      </c>
+      <c r="B94" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>24</v>
+      </c>
+      <c r="B95" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>24</v>
+      </c>
+      <c r="B96" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>24</v>
+      </c>
+      <c r="B97" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>24</v>
+      </c>
+      <c r="B98" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>24</v>
+      </c>
+      <c r="B99" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>24</v>
+      </c>
+      <c r="B100" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>24</v>
+      </c>
+      <c r="B101" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>24</v>
+      </c>
+      <c r="B102" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>24</v>
+      </c>
+      <c r="B103" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>24</v>
+      </c>
+      <c r="B104" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>24</v>
+      </c>
+      <c r="B105" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>24</v>
+      </c>
+      <c r="B106" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>24</v>
+      </c>
+      <c r="B107" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>24</v>
+      </c>
+      <c r="B108" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>24</v>
+      </c>
+      <c r="B109" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>24</v>
+      </c>
+      <c r="B110" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>24</v>
+      </c>
+      <c r="B111" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>24</v>
+      </c>
+      <c r="B112" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>24</v>
+      </c>
+      <c r="B113" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>24</v>
+      </c>
+      <c r="B114" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>24</v>
+      </c>
+      <c r="B115" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>24</v>
+      </c>
+      <c r="B116" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>24</v>
+      </c>
+      <c r="B117" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>24</v>
+      </c>
+      <c r="B118" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>24</v>
+      </c>
+      <c r="B119" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>24</v>
+      </c>
+      <c r="B120" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>24</v>
+      </c>
+      <c r="B121" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>